<commit_message>
Updated README.md, updated materials in Research dir
</commit_message>
<xml_diff>
--- a/research/content-inventory.xlsx
+++ b/research/content-inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leocast/Desktop/2023-repos/Portfolio/research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38F68DC-235C-BB4B-B4F7-DCCC2A59CD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14620F7-6BA8-E248-BD0F-B13844AA64E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="2260" windowWidth="21340" windowHeight="12880" xr2:uid="{722A7E64-0873-E84E-9FB6-DD3943D0F90F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Navigation Title</t>
   </si>
@@ -138,6 +138,21 @@
   </si>
   <si>
     <t>CMS Project</t>
+  </si>
+  <si>
+    <t>Tags: Project Management, UX Design</t>
+  </si>
+  <si>
+    <t>Tags: UX/UI Design</t>
+  </si>
+  <si>
+    <t>Tags: Project Management, UX/UI Design</t>
+  </si>
+  <si>
+    <t>Tags: Project Management, UX Design, Web Development</t>
+  </si>
+  <si>
+    <t>Work</t>
   </si>
 </sst>
 </file>
@@ -230,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -297,8 +312,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A194C1E-24E1-4149-93B0-C76C96D7FE33}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,7 +723,7 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>15</v>
@@ -749,7 +762,9 @@
       <c r="K4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -774,7 +789,9 @@
       <c r="K5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="5"/>
+      <c r="M5" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -799,7 +816,9 @@
       <c r="K6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -824,7 +843,9 @@
       <c r="K7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -992,39 +1013,32 @@
       <c r="A15" s="9">
         <v>6</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="30"/>
       <c r="E15" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="30"/>
       <c r="G15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="30"/>
       <c r="I15" s="25">
         <v>44973</v>
       </c>
-      <c r="J15" s="30"/>
       <c r="K15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="30"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="30"/>
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="E17" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>